<commit_message>
Added notes on workshops for 101
</commit_message>
<xml_diff>
--- a/DS101-Basic-Statistics/Workshops/8.1_v2-t-tests/weights_ttests.xlsx
+++ b/DS101-Basic-Statistics/Workshops/8.1_v2-t-tests/weights_ttests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dannylumian/Documents/GitHub/DS-Student-Resources/DS101-Basic-Statistics/Workshops/8.1_v2-t-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C72897-415E-AD42-83FD-BE3741391BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955723F5-7B06-EC47-9542-1F056236543D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{F65CD369-D53B-3545-BEDC-E28DDDD26522}"/>
+    <workbookView xWindow="3660" yWindow="2720" windowWidth="28040" windowHeight="17440" xr2:uid="{F65CD369-D53B-3545-BEDC-E28DDDD26522}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>